<commit_message>
Actualización de solicitud REC470
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/SolicitudGrafica_LE_08_02_REC470.xlsx
+++ b/fuentes/contenidos/grado08/guion02/SolicitudGrafica_LE_08_02_REC470.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AULA PLANETA\PROCESO JUNIO 2015\GRADO OCTAVO\LE_08_02_CO\AUTORIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AULA PLANETA\PROCESO JUNIO 2015\GRADO OCTAVO\LE_08_02_CO\MOTORES Y SOLICITUDES GRAFICAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="198">
   <si>
     <t>Fecha:</t>
   </si>
@@ -601,7 +601,31 @@
     <t>Fotografía</t>
   </si>
   <si>
-    <t>LE_08_02_REC440</t>
+    <t>LE_08_02_REC470</t>
+  </si>
+  <si>
+    <t>Un adorno barroco de filigrana</t>
+  </si>
+  <si>
+    <t>Tinta, pluma y un papiro antiguo</t>
+  </si>
+  <si>
+    <t>Una máquina de escribir antigua y un computador portátil</t>
+  </si>
+  <si>
+    <t>Una persona en un podio dando un discurso</t>
+  </si>
+  <si>
+    <t>Manos tecleando en un portátil</t>
+  </si>
+  <si>
+    <t>Una persona con una mano callándola</t>
+  </si>
+  <si>
+    <t>Unas ondas de audio</t>
+  </si>
+  <si>
+    <t>Alguien escribiendo en un teléfono celular</t>
   </si>
 </sst>
 </file>
@@ -2471,8 +2495,8 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2510,7 +2534,7 @@
       </c>
       <c r="M1" s="2" t="str">
         <f>CONCATENATE('Definición técnica de imagenes'!$B$1," ",$G$5)</f>
-        <v>Ubicación de la imagen en el recurso F13</v>
+        <v>Ubicación de la imagen en el recurso M101</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -2534,7 +2558,7 @@
       </c>
       <c r="M2" s="2" t="str">
         <f ca="1">IF($N2&lt;COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1+$N2,1,1,1),"")</f>
-        <v>Simple</v>
+        <v>Contenido</v>
       </c>
       <c r="N2" s="2">
         <v>0</v>
@@ -2550,7 +2574,7 @@
       </c>
       <c r="D3" s="85"/>
       <c r="F3" s="77">
-        <v>42241</v>
+        <v>42246</v>
       </c>
       <c r="G3" s="78"/>
       <c r="H3" s="58"/>
@@ -2561,7 +2585,7 @@
       </c>
       <c r="M3" s="2" t="str">
         <f ca="1">IF($N3&lt;COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1+$N3,1,1,1),"")</f>
-        <v>Doble</v>
+        <v/>
       </c>
       <c r="N3" s="2">
         <v>1</v>
@@ -2610,7 +2634,7 @@
         <v>Motor del recurso</v>
       </c>
       <c r="G5" s="61" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H5" s="58"/>
       <c r="I5" s="58"/>
@@ -2708,7 +2732,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>IF($G$4="Recurso",$M$1,$L$1)</f>
-        <v>Ubicación de la imagen en el recurso F13</v>
+        <v>Ubicación de la imagen en el recurso M101</v>
       </c>
       <c r="F9" s="57" t="s">
         <v>61</v>
@@ -2735,35 +2759,37 @@
         <v>IMG01</v>
       </c>
       <c r="B10" s="62">
-        <v>149746499</v>
+        <v>241975510</v>
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
-        <v>Recurso F13</v>
+        <v>Recurso M101</v>
       </c>
       <c r="D10" s="63" t="s">
         <v>188</v>
       </c>
       <c r="E10" s="63" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F10" s="13" t="str">
         <f t="shared" ref="F10" ca="1" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>LE_08_02_REC440_IMG01n.jpg</v>
+        <v>LE_08_02_REC470_IMG01n.png</v>
       </c>
       <c r="G10" s="13" t="str">
         <f ca="1">IF($F10&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 375 px</v>
+        <v>286 x 286 px</v>
       </c>
       <c r="H10" s="13" t="str">
         <f t="shared" ref="H10" ca="1" si="2">IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>LE_08_02_REC440_IMG01a.jpg</v>
+        <v>LE_08_02_REC470_IMG01a.png</v>
       </c>
       <c r="I10" s="13" t="str">
         <f ca="1">IF(OR($B10&lt;&gt;"",$J10&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="J10" s="63"/>
+        <v>500 x 500 px</v>
+      </c>
+      <c r="J10" s="63" t="s">
+        <v>190</v>
+      </c>
       <c r="K10" s="64"/>
     </row>
     <row r="11" spans="1:16" s="11" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2772,72 +2798,76 @@
         <v>IMG02</v>
       </c>
       <c r="B11" s="62">
-        <v>149746499</v>
+        <v>111836528</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso M101</v>
       </c>
       <c r="D11" s="63" t="s">
         <v>188</v>
       </c>
       <c r="E11" s="63" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F11" s="13" t="str">
         <f t="shared" ref="F11:F74" ca="1" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>LE_08_02_REC440_IMG02n.jpg</v>
+        <v>LE_08_02_REC470_IMG02n.png</v>
       </c>
       <c r="G11" s="13" t="str">
         <f ca="1">IF($F11&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v>286 x 286 px</v>
       </c>
       <c r="H11" s="13" t="str">
         <f t="shared" ref="H11:H74" ca="1" si="5">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>LE_08_02_REC440_IMG02a.jpg</v>
+        <v>LE_08_02_REC470_IMG02a.png</v>
       </c>
       <c r="I11" s="13" t="str">
         <f ca="1">IF(OR($B11&lt;&gt;"",$J11&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="J11" s="64"/>
+        <v>500 x 500 px</v>
+      </c>
+      <c r="J11" s="64" t="s">
+        <v>191</v>
+      </c>
       <c r="K11" s="65"/>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
       <c r="B12" s="62">
-        <v>293797889</v>
+        <v>185325812</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso M101</v>
       </c>
       <c r="D12" s="63" t="s">
         <v>188</v>
       </c>
       <c r="E12" s="63" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F12" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_08_02_REC440_IMG03n.jpg</v>
+        <v>LE_08_02_REC470_IMG03n.png</v>
       </c>
       <c r="G12" s="13" t="str">
         <f ca="1">IF($F12&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 375 px</v>
+        <v>286 x 286 px</v>
       </c>
       <c r="H12" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE_08_02_REC440_IMG03a.jpg</v>
+        <v>LE_08_02_REC470_IMG03a.png</v>
       </c>
       <c r="I12" s="13" t="str">
         <f ca="1">IF(OR($B12&lt;&gt;"",$J12&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="J12" s="64"/>
+        <v>500 x 500 px</v>
+      </c>
+      <c r="J12" s="64" t="s">
+        <v>192</v>
+      </c>
       <c r="K12" s="64"/>
     </row>
     <row r="13" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2846,35 +2876,37 @@
         <v>IMG04</v>
       </c>
       <c r="B13" s="62">
-        <v>293797889</v>
+        <v>200679422</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso M101</v>
       </c>
       <c r="D13" s="63" t="s">
         <v>188</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F13" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_08_02_REC440_IMG04n.jpg</v>
+        <v>LE_08_02_REC470_IMG04n.png</v>
       </c>
       <c r="G13" s="13" t="str">
         <f ca="1">IF($F13&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v>286 x 286 px</v>
       </c>
       <c r="H13" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE_08_02_REC440_IMG04a.jpg</v>
+        <v>LE_08_02_REC470_IMG04a.png</v>
       </c>
       <c r="I13" s="13" t="str">
         <f ca="1">IF(OR($B13&lt;&gt;"",$J13&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="J13" s="64"/>
+        <v>500 x 500 px</v>
+      </c>
+      <c r="J13" s="64" t="s">
+        <v>193</v>
+      </c>
       <c r="K13" s="64"/>
     </row>
     <row r="14" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2883,35 +2915,37 @@
         <v>IMG05</v>
       </c>
       <c r="B14" s="62">
-        <v>168161747</v>
+        <v>133973063</v>
       </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso M101</v>
       </c>
       <c r="D14" s="63" t="s">
         <v>188</v>
       </c>
       <c r="E14" s="63" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F14" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_08_02_REC440_IMG05n.jpg</v>
+        <v>LE_08_02_REC470_IMG05n.png</v>
       </c>
       <c r="G14" s="13" t="str">
         <f ca="1">IF($F14&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 375 px</v>
+        <v>286 x 286 px</v>
       </c>
       <c r="H14" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE_08_02_REC440_IMG05a.jpg</v>
+        <v>LE_08_02_REC470_IMG05a.png</v>
       </c>
       <c r="I14" s="13" t="str">
         <f ca="1">IF(OR($B14&lt;&gt;"",$J14&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="J14" s="64"/>
+        <v>500 x 500 px</v>
+      </c>
+      <c r="J14" s="64" t="s">
+        <v>194</v>
+      </c>
       <c r="K14" s="64"/>
     </row>
     <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2920,35 +2954,37 @@
         <v>IMG06</v>
       </c>
       <c r="B15" s="62">
-        <v>168161747</v>
+        <v>206286328</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso M101</v>
       </c>
       <c r="D15" s="63" t="s">
         <v>188</v>
       </c>
       <c r="E15" s="63" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F15" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_08_02_REC440_IMG06n.jpg</v>
+        <v>LE_08_02_REC470_IMG06n.png</v>
       </c>
       <c r="G15" s="13" t="str">
         <f ca="1">IF($F15&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v>286 x 286 px</v>
       </c>
       <c r="H15" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE_08_02_REC440_IMG06a.jpg</v>
+        <v>LE_08_02_REC470_IMG06a.png</v>
       </c>
       <c r="I15" s="13" t="str">
         <f ca="1">IF(OR($B15&lt;&gt;"",$J15&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="J15" s="66"/>
+        <v>500 x 500 px</v>
+      </c>
+      <c r="J15" s="66" t="s">
+        <v>195</v>
+      </c>
       <c r="K15" s="66"/>
     </row>
     <row r="16" spans="1:16" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
@@ -2957,33 +2993,37 @@
         <v>IMG07</v>
       </c>
       <c r="B16" s="62">
-        <v>116458489</v>
+        <v>128812483</v>
       </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
-      </c>
-      <c r="D16" s="63"/>
+        <v>Recurso M101</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>188</v>
+      </c>
       <c r="E16" s="63" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F16" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_08_02_REC440_IMG07n.jpg</v>
+        <v>LE_08_02_REC470_IMG07n.png</v>
       </c>
       <c r="G16" s="13" t="str">
         <f ca="1">IF($F16&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 375 px</v>
+        <v>286 x 286 px</v>
       </c>
       <c r="H16" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE_08_02_REC440_IMG07a.jpg</v>
+        <v>LE_08_02_REC470_IMG07a.png</v>
       </c>
       <c r="I16" s="13" t="str">
         <f ca="1">IF(OR($B16&lt;&gt;"",$J16&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="J16" s="67"/>
+        <v>500 x 500 px</v>
+      </c>
+      <c r="J16" s="67" t="s">
+        <v>196</v>
+      </c>
       <c r="K16" s="68"/>
     </row>
     <row r="17" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2992,66 +3032,66 @@
         <v>IMG08</v>
       </c>
       <c r="B17" s="62">
-        <v>116458489</v>
+        <v>167852012</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
-      </c>
-      <c r="D17" s="63"/>
+        <v>Recurso M101</v>
+      </c>
+      <c r="D17" s="63" t="s">
+        <v>188</v>
+      </c>
       <c r="E17" s="63" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F17" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_08_02_REC440_IMG08n.jpg</v>
+        <v>LE_08_02_REC470_IMG08n.png</v>
       </c>
       <c r="G17" s="13" t="str">
         <f ca="1">IF($F17&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v>286 x 286 px</v>
       </c>
       <c r="H17" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE_08_02_REC440_IMG08a.jpg</v>
+        <v>LE_08_02_REC470_IMG08a.png</v>
       </c>
       <c r="I17" s="13" t="str">
         <f ca="1">IF(OR($B17&lt;&gt;"",$J17&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="J17" s="66"/>
+        <v>500 x 500 px</v>
+      </c>
+      <c r="J17" s="66" t="s">
+        <v>197</v>
+      </c>
       <c r="K17" s="66"/>
     </row>
     <row r="18" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>IMG09</v>
-      </c>
-      <c r="B18" s="62">
-        <v>211996828</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B18" s="62"/>
       <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v/>
       </c>
       <c r="D18" s="63"/>
-      <c r="E18" s="63" t="s">
-        <v>153</v>
-      </c>
+      <c r="E18" s="63"/>
       <c r="F18" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>LE_08_02_REC440_IMG09n.jpg</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="G18" s="13" t="str">
         <f ca="1">IF($F18&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 375 px</v>
+        <v/>
       </c>
       <c r="H18" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE_08_02_REC440_IMG09a.jpg</v>
+        <v/>
       </c>
       <c r="I18" s="13" t="str">
         <f ca="1">IF(OR($B18&lt;&gt;"",$J18&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
+        <v/>
       </c>
       <c r="J18" s="66"/>
       <c r="K18" s="66"/>
@@ -3059,34 +3099,30 @@
     <row r="19" spans="1:11" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="str">
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
-        <v>IMG10</v>
-      </c>
-      <c r="B19" s="62">
-        <v>211996828</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B19" s="62"/>
       <c r="C19" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v/>
       </c>
       <c r="D19" s="63"/>
-      <c r="E19" s="63" t="s">
-        <v>154</v>
-      </c>
+      <c r="E19" s="63"/>
       <c r="F19" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>LE_08_02_REC440_IMG10n.jpg</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="G19" s="13" t="str">
         <f ca="1">IF($F19&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v/>
       </c>
       <c r="H19" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE_08_02_REC440_IMG10a.jpg</v>
+        <v/>
       </c>
       <c r="I19" s="13" t="str">
         <f ca="1">IF(OR($B19&lt;&gt;"",$J19&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
+        <v/>
       </c>
       <c r="J19" s="67"/>
       <c r="K19" s="68"/>
@@ -3094,34 +3130,30 @@
     <row r="20" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="str">
         <f t="shared" si="6"/>
-        <v>IMG11</v>
-      </c>
-      <c r="B20" s="62">
-        <v>256901572</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B20" s="62"/>
       <c r="C20" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v/>
       </c>
       <c r="D20" s="63"/>
-      <c r="E20" s="63" t="s">
-        <v>153</v>
-      </c>
+      <c r="E20" s="63"/>
       <c r="F20" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>LE_08_02_REC440_IMG11n.jpg</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="G20" s="13" t="str">
         <f ca="1">IF($F20&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 375 px</v>
+        <v/>
       </c>
       <c r="H20" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE_08_02_REC440_IMG11a.jpg</v>
+        <v/>
       </c>
       <c r="I20" s="13" t="str">
         <f ca="1">IF(OR($B20&lt;&gt;"",$J20&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
+        <v/>
       </c>
       <c r="J20" s="64"/>
       <c r="K20" s="66"/>
@@ -3129,34 +3161,30 @@
     <row r="21" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="str">
         <f t="shared" si="6"/>
-        <v>IMG12</v>
-      </c>
-      <c r="B21" s="62">
-        <v>256901572</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B21" s="62"/>
       <c r="C21" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v/>
       </c>
       <c r="D21" s="63"/>
-      <c r="E21" s="63" t="s">
-        <v>154</v>
-      </c>
+      <c r="E21" s="63"/>
       <c r="F21" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>LE_08_02_REC440_IMG12n.jpg</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="G21" s="13" t="str">
         <f ca="1">IF($F21&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v/>
       </c>
       <c r="H21" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE_08_02_REC440_IMG12a.jpg</v>
+        <v/>
       </c>
       <c r="I21" s="13" t="str">
         <f ca="1">IF(OR($B21&lt;&gt;"",$J21&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
+        <v/>
       </c>
       <c r="J21" s="66"/>
       <c r="K21" s="66"/>

</xml_diff>